<commit_message>
Add planilha com taxa de eficiência e super-eficiência (%)
</commit_message>
<xml_diff>
--- a/VN_DATA.xlsx
+++ b/VN_DATA.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Taxa de super-eficiencia" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="134">
   <si>
     <t>DMU</t>
   </si>
@@ -39,198 +40,6 @@
     <t>Hurst</t>
   </si>
   <si>
-    <t>DMU1</t>
-  </si>
-  <si>
-    <t>DMU2</t>
-  </si>
-  <si>
-    <t>DMU3</t>
-  </si>
-  <si>
-    <t>DMU4</t>
-  </si>
-  <si>
-    <t>DMU5</t>
-  </si>
-  <si>
-    <t>DMU6</t>
-  </si>
-  <si>
-    <t>DMU7</t>
-  </si>
-  <si>
-    <t>DMU8</t>
-  </si>
-  <si>
-    <t>DMU9</t>
-  </si>
-  <si>
-    <t>DMU10</t>
-  </si>
-  <si>
-    <t>DMU11</t>
-  </si>
-  <si>
-    <t>DMU12</t>
-  </si>
-  <si>
-    <t>DMU13</t>
-  </si>
-  <si>
-    <t>DMU14</t>
-  </si>
-  <si>
-    <t>DMU15</t>
-  </si>
-  <si>
-    <t>DMU16</t>
-  </si>
-  <si>
-    <t>DMU17</t>
-  </si>
-  <si>
-    <t>DMU18</t>
-  </si>
-  <si>
-    <t>DMU19</t>
-  </si>
-  <si>
-    <t>DMU20</t>
-  </si>
-  <si>
-    <t>DMU21</t>
-  </si>
-  <si>
-    <t>DMU22</t>
-  </si>
-  <si>
-    <t>DMU23</t>
-  </si>
-  <si>
-    <t>DMU24</t>
-  </si>
-  <si>
-    <t>DMU25</t>
-  </si>
-  <si>
-    <t>DMU26</t>
-  </si>
-  <si>
-    <t>DMU27</t>
-  </si>
-  <si>
-    <t>DMU28</t>
-  </si>
-  <si>
-    <t>DMU29</t>
-  </si>
-  <si>
-    <t>DMU30</t>
-  </si>
-  <si>
-    <t>DMU31</t>
-  </si>
-  <si>
-    <t>DMU32</t>
-  </si>
-  <si>
-    <t>DMU33</t>
-  </si>
-  <si>
-    <t>DMU34</t>
-  </si>
-  <si>
-    <t>DMU35</t>
-  </si>
-  <si>
-    <t>DMU36</t>
-  </si>
-  <si>
-    <t>DMU37</t>
-  </si>
-  <si>
-    <t>DMU38</t>
-  </si>
-  <si>
-    <t>DMU39</t>
-  </si>
-  <si>
-    <t>DMU40</t>
-  </si>
-  <si>
-    <t>DMU41</t>
-  </si>
-  <si>
-    <t>DMU42</t>
-  </si>
-  <si>
-    <t>DMU43</t>
-  </si>
-  <si>
-    <t>DMU44</t>
-  </si>
-  <si>
-    <t>DMU45</t>
-  </si>
-  <si>
-    <t>DMU46</t>
-  </si>
-  <si>
-    <t>DMU47</t>
-  </si>
-  <si>
-    <t>DMU48</t>
-  </si>
-  <si>
-    <t>DMU49</t>
-  </si>
-  <si>
-    <t>DMU50</t>
-  </si>
-  <si>
-    <t>DMU51</t>
-  </si>
-  <si>
-    <t>DMU52</t>
-  </si>
-  <si>
-    <t>DMU53</t>
-  </si>
-  <si>
-    <t>DMU54</t>
-  </si>
-  <si>
-    <t>DMU55</t>
-  </si>
-  <si>
-    <t>DMU56</t>
-  </si>
-  <si>
-    <t>DMU57</t>
-  </si>
-  <si>
-    <t>DMU58</t>
-  </si>
-  <si>
-    <t>DMU59</t>
-  </si>
-  <si>
-    <t>DMU60</t>
-  </si>
-  <si>
-    <t>DMU61</t>
-  </si>
-  <si>
-    <t>DMU62</t>
-  </si>
-  <si>
-    <t>DMU63</t>
-  </si>
-  <si>
-    <t>DMU64</t>
-  </si>
-  <si>
     <t xml:space="preserve">DMU2 </t>
   </si>
   <si>
@@ -418,6 +227,207 @@
   </si>
   <si>
     <t xml:space="preserve">DMU64 </t>
+  </si>
+  <si>
+    <t>DMU1   0.8264477</t>
+  </si>
+  <si>
+    <t>DMU2   0.7794651</t>
+  </si>
+  <si>
+    <t>DMU3   0.7942463</t>
+  </si>
+  <si>
+    <t>DMU4   0.9946474</t>
+  </si>
+  <si>
+    <t>DMU5   0.6543374</t>
+  </si>
+  <si>
+    <t>DMU6   0.7003361</t>
+  </si>
+  <si>
+    <t>DMU7   0.6141165</t>
+  </si>
+  <si>
+    <t>DMU8   0.9282931</t>
+  </si>
+  <si>
+    <t>DMU9   0.4910393</t>
+  </si>
+  <si>
+    <t>DMU10  0.6748607</t>
+  </si>
+  <si>
+    <t>DMU11  1.3385450</t>
+  </si>
+  <si>
+    <t>DMU12  0.5512170</t>
+  </si>
+  <si>
+    <t>DMU13  0.6630127</t>
+  </si>
+  <si>
+    <t>DMU14  0.6037125</t>
+  </si>
+  <si>
+    <t>DMU15  0.6748816</t>
+  </si>
+  <si>
+    <t>DMU16  0.9442271</t>
+  </si>
+  <si>
+    <t>DMU17  0.6265232</t>
+  </si>
+  <si>
+    <t>DMU18  0.6344359</t>
+  </si>
+  <si>
+    <t>DMU19  0.6656826</t>
+  </si>
+  <si>
+    <t>DMU20  0.6703364</t>
+  </si>
+  <si>
+    <t>DMU21  0.8034826</t>
+  </si>
+  <si>
+    <t>DMU22  0.7571107</t>
+  </si>
+  <si>
+    <t>DMU23  1.0777285</t>
+  </si>
+  <si>
+    <t>DMU24  0.6831996</t>
+  </si>
+  <si>
+    <t>DMU25  0.6828337</t>
+  </si>
+  <si>
+    <t>DMU26  0.6670358</t>
+  </si>
+  <si>
+    <t>DMU27  0.7046929</t>
+  </si>
+  <si>
+    <t>DMU28  0.5136543</t>
+  </si>
+  <si>
+    <t>DMU29  0.8956430</t>
+  </si>
+  <si>
+    <t>DMU30  0.7738368</t>
+  </si>
+  <si>
+    <t>DMU31  0.6797122</t>
+  </si>
+  <si>
+    <t>DMU32  0.4990573</t>
+  </si>
+  <si>
+    <t>DMU33  0.9547624</t>
+  </si>
+  <si>
+    <t>DMU34  0.7530345</t>
+  </si>
+  <si>
+    <t>DMU35  0.8085167</t>
+  </si>
+  <si>
+    <t>DMU36  0.6975310</t>
+  </si>
+  <si>
+    <t>DMU37  0.8200746</t>
+  </si>
+  <si>
+    <t>DMU38  0.7504360</t>
+  </si>
+  <si>
+    <t>DMU39  0.7457676</t>
+  </si>
+  <si>
+    <t>DMU40  0.4768937</t>
+  </si>
+  <si>
+    <t>DMU41  0.5738331</t>
+  </si>
+  <si>
+    <t>DMU42  0.5364931</t>
+  </si>
+  <si>
+    <t>DMU43  0.6064591</t>
+  </si>
+  <si>
+    <t>DMU44  0.6035406</t>
+  </si>
+  <si>
+    <t>DMU45  0.5748640</t>
+  </si>
+  <si>
+    <t>DMU46  0.6238163</t>
+  </si>
+  <si>
+    <t>DMU47  0.7465842</t>
+  </si>
+  <si>
+    <t>DMU48  0.7285226</t>
+  </si>
+  <si>
+    <t>DMU49  0.6445672</t>
+  </si>
+  <si>
+    <t>DMU50  0.7945605</t>
+  </si>
+  <si>
+    <t>DMU51  0.6257897</t>
+  </si>
+  <si>
+    <t>DMU52  0.9294849</t>
+  </si>
+  <si>
+    <t>DMU53  0.5890651</t>
+  </si>
+  <si>
+    <t>DMU54  0.5337387</t>
+  </si>
+  <si>
+    <t>DMU55  0.6931916</t>
+  </si>
+  <si>
+    <t>DMU56  0.5108932</t>
+  </si>
+  <si>
+    <t>DMU57  0.8258489</t>
+  </si>
+  <si>
+    <t>DMU58  0.7216367</t>
+  </si>
+  <si>
+    <t>DMU59  0.8181483</t>
+  </si>
+  <si>
+    <t>DMU60  0.7655479</t>
+  </si>
+  <si>
+    <t>DMU61  0.7278312</t>
+  </si>
+  <si>
+    <t>DMU62  0.7476861</t>
+  </si>
+  <si>
+    <t>DMU63  0.7931234</t>
+  </si>
+  <si>
+    <t>DMU64  0.7102271</t>
+  </si>
+  <si>
+    <t>Eficiencia</t>
+  </si>
+  <si>
+    <t>Super-eficiência</t>
+  </si>
+  <si>
+    <t>DMUs/DEA Results</t>
   </si>
 </sst>
 </file>
@@ -427,7 +437,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,6 +460,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -468,10 +493,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -491,9 +517,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +847,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
@@ -833,7 +862,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4">
         <v>1.7707120000000001</v>
@@ -847,7 +876,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4">
         <v>1.5582640000000001</v>
@@ -861,7 +890,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4">
         <v>2</v>
@@ -875,7 +904,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4">
         <v>1.9342299999999999</v>
@@ -889,7 +918,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4">
         <v>1.996229</v>
@@ -903,7 +932,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4">
         <v>1.6653439999999999</v>
@@ -917,7 +946,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
@@ -931,7 +960,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="B11" s="4">
         <v>1.860857</v>
@@ -945,7 +974,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4">
         <v>1.732553</v>
@@ -959,7 +988,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="B13" s="4">
         <v>1.9049370000000001</v>
@@ -973,7 +1002,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4">
         <v>1.931481</v>
@@ -987,7 +1016,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="B15" s="4">
         <v>1.900739</v>
@@ -1001,7 +1030,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="B16" s="4">
         <v>1.9361969999999999</v>
@@ -1015,7 +1044,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B17" s="4">
         <v>1.7771889999999999</v>
@@ -1029,7 +1058,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B18" s="4">
         <v>1.827153</v>
@@ -1043,7 +1072,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4">
         <v>1.802271</v>
@@ -1057,7 +1086,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4">
         <v>1.865664</v>
@@ -1071,7 +1100,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="B21" s="4">
         <v>1.9464030000000001</v>
@@ -1085,7 +1114,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="B22" s="4">
         <v>1.779212</v>
@@ -1099,7 +1128,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="B23" s="4">
         <v>1.6781980000000001</v>
@@ -1113,7 +1142,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="B24" s="4">
         <v>1.5693029999999999</v>
@@ -1127,7 +1156,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="B25" s="4">
         <v>1.920118</v>
@@ -1141,7 +1170,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="B26" s="4">
         <v>1.7232160000000001</v>
@@ -1155,7 +1184,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="B27" s="4">
         <v>1.889419</v>
@@ -1169,7 +1198,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="B28" s="4">
         <v>1.9970330000000001</v>
@@ -1183,7 +1212,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="B29" s="4">
         <v>1.9925919999999999</v>
@@ -1197,7 +1226,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="B30" s="4">
         <v>1.7286550000000001</v>
@@ -1211,7 +1240,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="B31" s="4">
         <v>1.655008</v>
@@ -1225,7 +1254,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="B32" s="4">
         <v>1.7907310000000001</v>
@@ -1239,7 +1268,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="B33" s="4">
         <v>1.75678</v>
@@ -1253,7 +1282,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="B34" s="4">
         <v>1.7509129999999999</v>
@@ -1267,7 +1296,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>100</v>
+        <v>36</v>
       </c>
       <c r="B35" s="4">
         <v>1.9994369999999999</v>
@@ -1281,7 +1310,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="B36" s="4">
         <v>1.9873499999999999</v>
@@ -1295,7 +1324,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="B37" s="4">
         <v>1.949573</v>
@@ -1309,7 +1338,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="B38" s="4">
         <v>1.7094609999999999</v>
@@ -1323,7 +1352,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="B39" s="4">
         <v>1.7587619999999999</v>
@@ -1337,7 +1366,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="B40" s="4">
         <v>2</v>
@@ -1351,7 +1380,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="B41" s="4">
         <v>1.974318</v>
@@ -1365,7 +1394,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
       <c r="B42" s="4">
         <v>1.936423</v>
@@ -1379,7 +1408,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B43" s="4">
         <v>1.9805120000000001</v>
@@ -1393,7 +1422,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
       <c r="B44" s="4">
         <v>1.8767309999999999</v>
@@ -1407,7 +1436,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="B45" s="4">
         <v>1.7485390000000001</v>
@@ -1421,7 +1450,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="B46" s="4">
         <v>1.884171</v>
@@ -1435,7 +1464,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="B47" s="4">
         <v>1.9563569999999999</v>
@@ -1449,7 +1478,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="B48" s="4">
         <v>1.9827900000000001</v>
@@ -1463,7 +1492,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="B49" s="4">
         <v>1.9764200000000001</v>
@@ -1477,7 +1506,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>115</v>
+        <v>51</v>
       </c>
       <c r="B50" s="4">
         <v>1.7321869999999999</v>
@@ -1491,7 +1520,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="B51" s="4">
         <v>1.838379</v>
@@ -1505,7 +1534,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="B52" s="4">
         <v>1.9158850000000001</v>
@@ -1519,7 +1548,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>118</v>
+        <v>54</v>
       </c>
       <c r="B53" s="4">
         <v>1.629499</v>
@@ -1533,7 +1562,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="B54" s="4">
         <v>1.9029990000000001</v>
@@ -1547,7 +1576,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="B55" s="4">
         <v>2</v>
@@ -1561,7 +1590,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>121</v>
+        <v>57</v>
       </c>
       <c r="B56" s="4">
         <v>1.918404</v>
@@ -1575,7 +1604,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="B57" s="4">
         <v>1.8430310000000001</v>
@@ -1589,7 +1618,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="B58" s="4">
         <v>1.7239599999999999</v>
@@ -1603,7 +1632,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="B59" s="4">
         <v>1.7388269999999999</v>
@@ -1617,7 +1646,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="B60" s="4">
         <v>1.69848</v>
@@ -1631,7 +1660,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="B61" s="4">
         <v>1.8153779999999999</v>
@@ -1645,7 +1674,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B62" s="4">
         <v>1.865518</v>
@@ -1659,7 +1688,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="B63" s="4">
         <v>1.706896</v>
@@ -1673,7 +1702,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="B64" s="4">
         <v>1.833882</v>
@@ -1687,7 +1716,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B65" s="4">
         <v>1.675289</v>
@@ -1707,530 +1736,748 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6">
-        <v>5782.1170000000002</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6">
-        <v>5170.2809999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="B2" s="9">
+        <v>0.82</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6">
-        <v>13083.84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.77</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6">
-        <v>451532.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.79</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6">
-        <v>5766.66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.99</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6">
-        <v>6063.8940000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.65</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6">
-        <v>1477.5239999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6">
-        <v>355283</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.61</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="6">
-        <v>3506.2060000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.49</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="6">
-        <v>3491.5419999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0.49</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1236833</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.67</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="6">
-        <v>12480.43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="6">
-        <v>346853.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6">
-        <v>4428.29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="6">
-        <v>266279.09999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="6">
-        <v>290103.59999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.67</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6">
-        <v>3571.2240000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.94</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="6">
-        <v>3841.252</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="6">
-        <v>380867.4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.63</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="6">
-        <v>11599.28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="6">
-        <v>353692.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0.67</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="6">
-        <v>4625.1419999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="B22" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="6">
-        <v>2906.866</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="6">
-        <v>3380.2379999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="6">
-        <v>3895.4470000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="6">
-        <v>3552.2530000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="6">
-        <v>369954.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="6">
-        <v>9368.4969999999994</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="6">
-        <v>350665.3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="6">
-        <v>4609.51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="B30" s="9">
+        <v>0.89</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="6">
-        <v>498603.6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0.77</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="6">
-        <v>10972.66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="B32" s="9">
+        <v>0.67</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="6">
-        <v>593239.30000000005</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="B33" s="9">
+        <v>0.49</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="6">
-        <v>5525.0110000000004</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="B34" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="6">
-        <v>808516.7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="B35" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="C35" s="9">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="6">
-        <v>9237517000000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="B36" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="6">
-        <v>527111.6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="B37" s="9">
+        <v>0.69</v>
+      </c>
+      <c r="C37" s="9">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="6">
-        <v>6460.61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="B38" s="9">
+        <v>0.82</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="6">
-        <v>5511.174</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="B39" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="6">
-        <v>5839.0519999999997</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="B40" s="9">
+        <v>0.74</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="6">
-        <v>1749.886</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B41" s="9">
+        <v>0.47</v>
+      </c>
+      <c r="C41" s="9">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="6">
-        <v>3465.1190000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="B42" s="9">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="6">
-        <v>12238.01</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="B43" s="9">
+        <v>0.53</v>
+      </c>
+      <c r="C43" s="9">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="6">
-        <v>13118.76</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="B44" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="6">
-        <v>4333.8689999999997</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="B45" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="C45" s="9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="6">
-        <v>4385.9189999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="B46" s="9">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C46" s="9">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="6">
-        <v>257465.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="B47" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="C47" s="9">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="6">
-        <v>3194.6579999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="B48" s="9">
+        <v>0.74</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="6">
-        <v>3665.4270000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="B49" s="9">
+        <v>0.72</v>
+      </c>
+      <c r="C49" s="9">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="6">
-        <v>3625.9870000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="B50" s="9">
+        <v>0.64</v>
+      </c>
+      <c r="C50" s="9">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="6">
-        <v>265691.59999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="B51" s="9">
+        <v>0.79</v>
+      </c>
+      <c r="C51" s="9">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="6">
-        <v>10317.06</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="B52" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="C52" s="9">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="6">
-        <v>356081.9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="B53" s="9">
+        <v>0.92</v>
+      </c>
+      <c r="C53" s="9">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="6">
-        <v>4144.3140000000003</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="B54" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C54" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="6">
-        <v>282423.8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="B55" s="9">
+        <v>0.53</v>
+      </c>
+      <c r="C55" s="9">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" s="6">
-        <v>3521.8649999999998</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="B56" s="9">
+        <v>0.69</v>
+      </c>
+      <c r="C56" s="9">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" s="6">
-        <v>291866.09999999998</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="B57" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="C57" s="9">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
-      </c>
-      <c r="B58" s="6">
-        <v>2651.3240000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="B58" s="9">
+        <v>0.82</v>
+      </c>
+      <c r="C58" s="9">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>62</v>
-      </c>
-      <c r="B59" s="6">
-        <v>327677.09999999998</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="B59" s="9">
+        <v>0.72</v>
+      </c>
+      <c r="C59" s="9">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>63</v>
-      </c>
-      <c r="B60" s="6">
-        <v>3814.32</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="B60" s="9">
+        <v>0.81</v>
+      </c>
+      <c r="C60" s="9">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>64</v>
-      </c>
-      <c r="B61" s="6">
-        <v>347308.6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="B61" s="9">
+        <v>0.76</v>
+      </c>
+      <c r="C61" s="9">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" s="6">
-        <v>4828.9750000000004</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="B62" s="9">
+        <v>0.72</v>
+      </c>
+      <c r="C62" s="9">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" s="6">
-        <v>3457.346</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="B63" s="9">
+        <v>0.74</v>
+      </c>
+      <c r="C63" s="9">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>67</v>
-      </c>
-      <c r="B64" s="6">
-        <v>4157.4189999999999</v>
+        <v>129</v>
+      </c>
+      <c r="B64" s="9">
+        <v>0.79</v>
+      </c>
+      <c r="C64" s="9">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="9">
+        <v>0.71</v>
+      </c>
+      <c r="C65" s="9">
+        <v>0.71</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>